<commit_message>
Conditionally include hazard information in location description in updateUI method
- Modified the `updateUI` method to append hazard information to the location description only if a hazard exists.
- Ensured hazard details are checked for validity before being added.
- Retained the functionality for updating player status and available actions.
- Improved clarity and conditional logic for hazard handling.
- Edited my product and sprint backlog.
</commit_message>
<xml_diff>
--- a/documentation/Product Backlog.xlsx
+++ b/documentation/Product Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcorley\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ne00040\Desktop\TextAdventureGame\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74866A28-4BAB-4A0A-B5C3-34B3C6CF265C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F4383F-7453-499E-ACE0-3E33AEDFFDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -169,12 +169,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -190,6 +197,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/featurePropertyBag/featurePropertyBag.xml><?xml version="1.0" encoding="utf-8"?>
+<FeaturePropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag">
+  <bag type="Checkbox"/>
+  <bag type="XFControls">
+    <bagId k="CellControl">0</bagId>
+  </bag>
+  <bag type="XFComplement">
+    <bagId k="XFControls">1</bagId>
+  </bag>
+  <bag type="XFComplements" extRef="XFComplementsMapperExtRef">
+    <a k="MappedFeaturePropertyBags">
+      <bagId>2</bagId>
+    </a>
+  </bag>
+</FeaturePropertyBags>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -457,20 +481,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.5546875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -487,8 +511,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
@@ -502,8 +528,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="B3" s="3">
         <v>1</v>
       </c>
@@ -517,8 +545,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="B4" s="3">
         <v>1</v>
       </c>
@@ -532,8 +562,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="B5" s="3">
         <v>1</v>
       </c>
@@ -547,7 +579,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3">
         <v>2</v>
@@ -562,7 +594,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3">
         <v>2</v>
@@ -577,7 +609,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3">
         <v>2</v>
@@ -592,7 +624,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3">
         <v>3</v>
@@ -607,35 +639,35 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>

</xml_diff>